<commit_message>
export estimation resource count api done
</commit_message>
<xml_diff>
--- a/backend/report/Estimation_SWAG-Dell-Test_Project_phase1.xlsx
+++ b/backend/report/Estimation_SWAG-Dell-Test_Project_phase1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Tag</t>
   </si>
@@ -74,7 +74,7 @@
     <t>Python</t>
   </si>
   <si>
-    <t/>
+    <t>25 Lead,20 Sr Lead</t>
   </si>
   <si>
     <t>4.50</t>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Node API</t>
+  </si>
+  <si>
+    <t>3 Sr Lead,2 Lead</t>
   </si>
 </sst>
 </file>
@@ -670,7 +673,7 @@
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>